<commit_message>
Change Grade Evaluation Logic v1
</commit_message>
<xml_diff>
--- a/sctkpy/templates/grade_report_template.xlsx
+++ b/sctkpy/templates/grade_report_template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Study Hours" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Study Hours'!$L$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Study Hours'!$N$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,15 +23,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Pledge Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prev. Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prev. GPA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pledge Class</t>
   </si>
   <si>
     <t xml:space="preserve">Term GPA</t>
@@ -632,23 +638,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="23.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="11.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="23.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="23.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="4" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,230 +673,236 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="J2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="6"/>
-      <c r="G3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F4" s="6"/>
-      <c r="G4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="3"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="6"/>
-      <c r="G5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="3"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="6"/>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="6"/>
+      <c r="I7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="6"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="6"/>
+      <c r="I9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="6"/>
+      <c r="I10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="6"/>
-      <c r="G7" s="13" t="s">
+      <c r="J10" s="12"/>
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="6"/>
+      <c r="I11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="6"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="6"/>
-      <c r="G9" s="16" t="s">
+      <c r="J11" s="14"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="6"/>
+      <c r="I12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="6"/>
-      <c r="G10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="6"/>
-      <c r="G11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="6"/>
-      <c r="G12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="11"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F13" s="6"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="6"/>
-      <c r="G14" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="6"/>
-      <c r="G15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="11"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F17" s="6"/>
-      <c r="G17" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="18"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F19" s="6"/>
-      <c r="G19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="6"/>
-      <c r="G20" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>20</v>
-      </c>
+      <c r="H20" s="6"/>
       <c r="I20" s="19" t="s">
         <v>21</v>
       </c>
+      <c r="J20" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="6"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="6"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="6"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
       <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
       <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
       <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
       <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
       <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="I1:K1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I19:K19"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:E101">
+  <conditionalFormatting sqref="A2:G101">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>AND($D2 &lt; $F$4, $D2  &gt;= $F$5,  $A2&lt;&gt;"", $D2&lt;&gt;"")</formula>
+      <formula>AND($F2 &lt; $H$4, $F2  &gt;= $H$5,  $A2&lt;&gt;"", $F2&lt;&gt;"")</formula>
     </cfRule>
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($D2  &lt; $F$5, $A2&lt;&gt;"", $D2&lt;&gt;"")</formula>
+      <formula>AND($F2  &lt; $H$5, $A2&lt;&gt;"", $F2&lt;&gt;"")</formula>
     </cfRule>
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND(ISODD(ROW())=1, ROW()&gt;=2, AND(COLUMN(1:1)), $A2&lt;&gt;"")</formula>

</xml_diff>

<commit_message>
Updated Study Hour Evaluation Logic.
</commit_message>
<xml_diff>
--- a/sctkpy/templates/grade_report_template.xlsx
+++ b/sctkpy/templates/grade_report_template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Study Hours" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Study Hours'!$N$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Study Hours'!$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Pledge Class</t>
   </si>
   <si>
+    <t xml:space="preserve">Cum. GPA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prev. Term</t>
   </si>
   <si>
@@ -82,6 +85,33 @@
     <t xml:space="preserve">So-Pro Placeholder Text</t>
   </si>
   <si>
+    <t xml:space="preserve">Academic Suspension Placeholder Text (TERM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Academic Suspension Placeholder Text (CUMULATIVE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduce Study Hour Sanctions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term GPA Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumulative GPA Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduce One-Tier Placeholder Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduce Two-Tier Placeholder Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduce No Punting Placeholder Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduce Social Probation Placeholder Text</t>
+  </si>
+  <si>
     <t xml:space="preserve">House Average GPA:</t>
   </si>
   <si>
@@ -94,7 +124,13 @@
     <t xml:space="preserve"># Members</t>
   </si>
   <si>
-    <t xml:space="preserve">Avg. GPA</t>
+    <t xml:space="preserve">Avg GPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rank</t>
   </si>
 </sst>
 </file>
@@ -105,7 +141,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -136,6 +172,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -251,7 +295,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,6 +309,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,7 +324,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -304,6 +352,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -312,7 +364,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -320,6 +372,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -328,12 +392,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -638,271 +698,595 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="23.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="11.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="23.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.09"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="11.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="10" style="5" width="11.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="15" style="5" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="N2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H3" s="6"/>
-      <c r="I3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H4" s="6"/>
-      <c r="I4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="3"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H5" s="6"/>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I6" s="7"/>
+      <c r="J6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="7"/>
+      <c r="J7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="7"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I9" s="7"/>
+      <c r="J9" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="7"/>
+      <c r="J10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="6"/>
-      <c r="I6" s="13" t="s">
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="7"/>
+      <c r="J11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H7" s="6"/>
-      <c r="I7" s="13" t="s">
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I12" s="7"/>
+      <c r="J12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H8" s="6"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H9" s="6"/>
-      <c r="I9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H10" s="6"/>
-      <c r="I10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H11" s="6"/>
-      <c r="I11" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H12" s="6"/>
-      <c r="I12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="11"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H13" s="6"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="6"/>
-      <c r="I14" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="6"/>
-      <c r="I15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="11"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="6"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="6"/>
-      <c r="I17" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="18"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="6"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="6"/>
-      <c r="I19" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="6"/>
-      <c r="I20" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20" s="19" t="s">
+      <c r="I20" s="7"/>
+      <c r="J20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="6"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="K21" s="20"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="6"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="14"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="6"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="14"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="7"/>
+      <c r="J29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I30" s="7"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="21"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I31" s="7"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="21"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="7"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="21"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="21"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="21"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="21"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="21"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="21"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="21"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="21"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="21"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="21"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="21"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="21"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="21"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="21"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="21"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="21"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="21"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="21"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I19:K19"/>
+  <mergeCells count="48">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="J28:O28"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:G101">
+  <conditionalFormatting sqref="A2:H110">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>AND($F2 &lt; $H$4, $F2  &gt;= $H$5,  $A2&lt;&gt;"", $F2&lt;&gt;"")</formula>
+      <formula>AND($G2 &lt; $I$4, $G2  &gt;= $I$5,  $A2&lt;&gt;"", $G2&lt;&gt;"")</formula>
     </cfRule>
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($F2  &lt; $H$5, $A2&lt;&gt;"", $F2&lt;&gt;"")</formula>
+      <formula>AND($G2  &lt; $I$5, $A2&lt;&gt;"", $G2&lt;&gt;"")</formula>
     </cfRule>
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>AND(ISODD(ROW())=1, ROW()&gt;=2, AND(COLUMN(1:1)), $A2&lt;&gt;"")</formula>

</xml_diff>